<commit_message>
data pelanggan per petugas
</commit_message>
<xml_diff>
--- a/import/Format Import Tusbung Harian.xlsx
+++ b/import/Format Import Tusbung Harian.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp7\htdocs\billmanplnt\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D1D04D-58AD-4DBC-8AAC-B03E110A9C37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12BCB827-025B-4370-BBD5-BBC5A23A68CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15750" xr2:uid="{AFDB4832-0DB3-4261-BED5-0029AE39DDBF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{AFDB4832-0DB3-4261-BED5-0029AE39DDBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="30">
   <si>
     <t>idpel</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>diinput tapi dicek dulu idpel di data pelanggan dan tusbung kumulatif berdasarkan bulan dan tahun</t>
+  </si>
+  <si>
+    <t>di cek petugas sesuai data di petugas, dan di tusbung kumulatif</t>
   </si>
 </sst>
 </file>
@@ -334,23 +337,23 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{15CC70B9-751C-424F-9086-BBC6732F895D}"/>
     <cellStyle name="Normal 2 4" xfId="2" xr:uid="{4A7D5451-36AF-4D1D-999A-A041640C7749}"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -363,13 +366,6 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
@@ -691,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AC61CD2-87A3-4ECB-82A5-1B02BF637F9B}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -817,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB29B3C9-E913-4EE3-BCF0-E276CF08FE29}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -832,10 +828,10 @@
     <col min="7" max="7" width="20.7109375" style="20" customWidth="1"/>
     <col min="8" max="8" width="17.7109375" style="7" customWidth="1"/>
     <col min="9" max="9" width="18.42578125" style="7" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" style="20" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" style="24" customWidth="1"/>
     <col min="11" max="11" width="9.140625" style="7"/>
     <col min="12" max="12" width="13.5703125" style="20" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" style="22" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" customWidth="1"/>
     <col min="14" max="14" width="12.7109375" style="20" customWidth="1"/>
     <col min="15" max="15" width="10.7109375" style="20" customWidth="1"/>
     <col min="16" max="16" width="18.85546875" customWidth="1"/>
@@ -869,7 +865,7 @@
       <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="5" t="s">
@@ -878,10 +874,10 @@
       <c r="L1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="M1" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="24" t="s">
+      <c r="N1" s="22" t="s">
         <v>16</v>
       </c>
       <c r="O1" s="18" t="s">
@@ -919,8 +915,8 @@
       <c r="I2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>14</v>
+      <c r="J2" s="23" t="s">
+        <v>29</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>14</v>
@@ -928,7 +924,7 @@
       <c r="L2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="21" t="s">
+      <c r="M2" s="4" t="s">
         <v>26</v>
       </c>
       <c r="N2" s="19" t="s">
@@ -937,7 +933,7 @@
       <c r="O2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="21" t="s">
+      <c r="P2" s="4" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update lunas blm selesai
</commit_message>
<xml_diff>
--- a/import/Format Import Tusbung Harian.xlsx
+++ b/import/Format Import Tusbung Harian.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp7\htdocs\billmanplnt\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12BCB827-025B-4370-BBD5-BBC5A23A68CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2132A1D8-F8B2-47B9-B63E-719E28855C9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{AFDB4832-0DB3-4261-BED5-0029AE39DDBF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{AFDB4832-0DB3-4261-BED5-0029AE39DDBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -133,7 +133,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,7 +285,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -343,10 +343,6 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -687,17 +683,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AC61CD2-87A3-4ECB-82A5-1B02BF637F9B}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="13" max="13" width="19.140625" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="31.5">
+    <row r="1" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -747,7 +744,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>424110008581</v>
       </c>
@@ -813,11 +810,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB29B3C9-E913-4EE3-BCF0-E276CF08FE29}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" style="20" customWidth="1"/>
@@ -828,7 +825,7 @@
     <col min="7" max="7" width="20.7109375" style="20" customWidth="1"/>
     <col min="8" max="8" width="17.7109375" style="7" customWidth="1"/>
     <col min="9" max="9" width="18.42578125" style="7" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" style="24" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" customWidth="1"/>
     <col min="11" max="11" width="9.140625" style="7"/>
     <col min="12" max="12" width="13.5703125" style="20" customWidth="1"/>
     <col min="13" max="13" width="16.85546875" customWidth="1"/>
@@ -837,7 +834,7 @@
     <col min="16" max="16" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="31.5">
+    <row r="1" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -887,7 +884,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="3" customFormat="1" ht="102.75" customHeight="1">
+    <row r="2" spans="1:16" s="3" customFormat="1" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>28</v>
       </c>
@@ -915,7 +912,7 @@
       <c r="I2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="4" t="s">
         <v>29</v>
       </c>
       <c r="K2" s="6" t="s">

</xml_diff>